<commit_message>
Chỉnh sửa phần import và thuật toán
</commit_message>
<xml_diff>
--- a/Template/dsnv.xlsx
+++ b/Template/dsnv.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="152511" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -341,9 +341,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -355,6 +352,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,55 +636,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E30"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
@@ -693,12 +711,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>16</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
@@ -710,15 +728,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>18</v>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>7</v>
@@ -727,29 +745,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>20</v>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>22</v>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
@@ -761,15 +779,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>24</v>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>12</v>
@@ -778,12 +796,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>26</v>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>11</v>
@@ -795,12 +813,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>28</v>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>11</v>
@@ -812,12 +830,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>30</v>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>11</v>
@@ -829,12 +847,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>32</v>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>11</v>
@@ -846,12 +864,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>34</v>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>11</v>
@@ -863,12 +881,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>36</v>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>11</v>
@@ -880,12 +898,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>38</v>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>11</v>
@@ -897,12 +915,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>40</v>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>11</v>
@@ -914,12 +932,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>42</v>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>11</v>
@@ -931,12 +949,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>44</v>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>11</v>
@@ -948,12 +966,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>46</v>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>11</v>
@@ -965,12 +983,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>48</v>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>11</v>
@@ -982,12 +1000,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>50</v>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>11</v>
@@ -999,12 +1017,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>52</v>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>11</v>
@@ -1016,12 +1034,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>54</v>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>11</v>
@@ -1033,12 +1051,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>56</v>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>11</v>
@@ -1050,12 +1068,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>58</v>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>11</v>
@@ -1067,12 +1085,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>11</v>
@@ -1084,12 +1102,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>11</v>
@@ -1101,12 +1119,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>64</v>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>11</v>
@@ -1115,29 +1133,12 @@
         <v>12</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="3" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>